<commit_message>
Refatoração e ajuste de detalhes
</commit_message>
<xml_diff>
--- a/excel/ExcelAppiumBdd.xlsx
+++ b/excel/ExcelAppiumBdd.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emerson.prado\eclipse-toolsqa\workspace-appium\AppiumBDD\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0620BC32-A1D9-414D-901C-E2322A3B9578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9365BD-361F-4385-93F3-C7FF81A7E4B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{EE607779-C7A4-4C40-B0F3-D8929BB2081C}"/>
   </bookViews>
   <sheets>
-    <sheet name="produtoCategoria" sheetId="1" r:id="rId1"/>
-    <sheet name="produtoTexto" sheetId="2" r:id="rId2"/>
+    <sheet name="produtos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Categoria</t>
   </si>
@@ -42,16 +41,16 @@
     <t>Produto</t>
   </si>
   <si>
-    <t>HP Z8000 BLUETOOTH MOUSE</t>
-  </si>
-  <si>
     <t>Pesquisa</t>
   </si>
   <si>
-    <t>mouse</t>
-  </si>
-  <si>
-    <t>MICE</t>
+    <t>LOGITECH USB HEADSET H390</t>
+  </si>
+  <si>
+    <t>HEADPHONES</t>
+  </si>
+  <si>
+    <t>HEADSET</t>
   </si>
 </sst>
 </file>
@@ -403,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2A8984-BFDF-430F-AB09-C172C64AA44C}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,19 +414,25 @@
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -435,38 +440,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473A7150-E195-4F28-AFCF-5CB232ED3AB7}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>